<commit_message>
Review more Coursera skills
</commit_message>
<xml_diff>
--- a/skills/Skills.xlsx
+++ b/skills/Skills.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Skills Ontology/skills/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kongbinxuan/Desktop/skills-onthology-project/skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB5CFB2-A5EF-6F49-9181-374D50AFC09F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE93378-4030-3148-BA44-469EBDC95A31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="460" windowWidth="13600" windowHeight="16140" activeTab="5" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="13600" windowHeight="16140" activeTab="5" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Parent 1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4052" uniqueCount="1701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4108" uniqueCount="1729">
   <si>
     <t>Skill</t>
   </si>
@@ -5143,6 +5143,90 @@
   </si>
   <si>
     <t>Artificial Intelligence (AI)</t>
+  </si>
+  <si>
+    <t>News Writing</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Financial Data Analysis</t>
+  </si>
+  <si>
+    <t>Environmental Data Analysis</t>
+  </si>
+  <si>
+    <t>Pricing Policy</t>
+  </si>
+  <si>
+    <t>Human Resource</t>
+  </si>
+  <si>
+    <t>Performance Management</t>
+  </si>
+  <si>
+    <t>Sociological Concept</t>
+  </si>
+  <si>
+    <t>Economic Analysis</t>
+  </si>
+  <si>
+    <t>Economic Models</t>
+  </si>
+  <si>
+    <t>Business Analysis</t>
+  </si>
+  <si>
+    <t>Intellectual Property</t>
+  </si>
+  <si>
+    <t>Google Chart API</t>
+  </si>
+  <si>
+    <t>Google Services</t>
+  </si>
+  <si>
+    <t>Policy</t>
+  </si>
+  <si>
+    <t>Uniform Resource Identifier (URI) Scheme</t>
+  </si>
+  <si>
+    <t>Financial Risk Modeling</t>
+  </si>
+  <si>
+    <t>RStudio</t>
+  </si>
+  <si>
+    <t>Auditor's Report</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>Data Reporting</t>
+  </si>
+  <si>
+    <t>Sales Presentation</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Sales Management</t>
+  </si>
+  <si>
+    <t>Software Stack</t>
+  </si>
+  <si>
+    <t>Business Technology Management</t>
+  </si>
+  <si>
+    <t>Market Analysis</t>
+  </si>
+  <si>
+    <t>Cloud Computing Security</t>
   </si>
 </sst>
 </file>
@@ -5783,7 +5867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55E440C-1904-894B-9323-83431D3F77DA}">
   <dimension ref="A1:B168"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
@@ -15923,8 +16007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99003BE-679F-9248-8C84-529C7407F5E3}">
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16402,6 +16486,230 @@
       </c>
       <c r="B59" t="s">
         <v>443</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B61" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B62" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B66" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B67" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B68" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B76" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B77" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B85" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B87" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Map coursera skills to skills
</commit_message>
<xml_diff>
--- a/skills/Skills.xlsx
+++ b/skills/Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Skills Ontology/skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66B5821-7F81-6847-9B25-276839B8E8AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D369AF08-1D57-684C-BC7B-8E5F871ACB14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="13600" windowHeight="16140" activeTab="5" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4222" uniqueCount="1791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4268" uniqueCount="1810">
   <si>
     <t>Skill</t>
   </si>
@@ -5178,9 +5178,6 @@
     <t>Business Analysis</t>
   </si>
   <si>
-    <t>Intellectual Property</t>
-  </si>
-  <si>
     <t>Google Chart API</t>
   </si>
   <si>
@@ -5316,9 +5313,6 @@
     <t>Kubernetes</t>
   </si>
   <si>
-    <t>Infrastructure as a Serivce (IaaS)</t>
-  </si>
-  <si>
     <t>Social Media Analytics</t>
   </si>
   <si>
@@ -5413,6 +5407,69 @@
   </si>
   <si>
     <t>Video Game Graphics</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Bond</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Computer-aided Design</t>
+  </si>
+  <si>
+    <t>Data Language</t>
+  </si>
+  <si>
+    <t>Decision Process</t>
+  </si>
+  <si>
+    <t>Differentiation</t>
+  </si>
+  <si>
+    <t>Event Processor</t>
+  </si>
+  <si>
+    <t>Processor</t>
+  </si>
+  <si>
+    <t>Mathematical Function</t>
+  </si>
+  <si>
+    <t>Mechanics</t>
+  </si>
+  <si>
+    <t>Open Access Network (OAN)</t>
+  </si>
+  <si>
+    <t>Securities</t>
+  </si>
+  <si>
+    <t>Scripting</t>
+  </si>
+  <si>
+    <t>Hospitality</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Security Exploit</t>
+  </si>
+  <si>
+    <t>Production Process</t>
+  </si>
+  <si>
+    <t>Systems Development</t>
+  </si>
+  <si>
+    <t>Web Server Software</t>
+  </si>
+  <si>
+    <t>Web Server</t>
   </si>
 </sst>
 </file>
@@ -5530,8 +5587,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5EC86AD1-B64A-EF4A-9E30-4E59C5D34B29}" name="Table3" displayName="Table3" ref="A1:B168" totalsRowShown="0">
-  <autoFilter ref="A1:B168" xr:uid="{2DF645BF-484A-D846-BB3C-AFD56E1950FF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5EC86AD1-B64A-EF4A-9E30-4E59C5D34B29}" name="Table3" displayName="Table3" ref="A1:B170" totalsRowShown="0">
+  <autoFilter ref="A1:B170" xr:uid="{2DF645BF-484A-D846-BB3C-AFD56E1950FF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B168">
     <sortCondition ref="A1:A168"/>
   </sortState>
@@ -5586,10 +5643,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BD7CD51A-AB5A-EF4F-92CB-40C5D2E89560}" name="Table4678" displayName="Table4678" ref="A1:B145" totalsRowShown="0">
-  <autoFilter ref="A1:B145" xr:uid="{87A65D69-75EC-4A48-9B55-77C093F67BDB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B97">
-    <sortCondition ref="A1:A97"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BD7CD51A-AB5A-EF4F-92CB-40C5D2E89560}" name="Table4678" displayName="Table4678" ref="A1:B166" totalsRowShown="0">
+  <autoFilter ref="A1:B166" xr:uid="{87A65D69-75EC-4A48-9B55-77C093F67BDB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B159">
+    <sortCondition ref="B1:B159"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C60D6BEC-005F-9346-9865-1C2241A1B490}" name="Skill"/>
@@ -6051,10 +6108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55E440C-1904-894B-9323-83431D3F77DA}">
-  <dimension ref="A1:B168"/>
+  <dimension ref="A1:B170"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7404,6 +7461,22 @@
       </c>
       <c r="B168" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B169" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B170" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -7418,8 +7491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F7A090-657A-7848-AF08-37C999ED8681}">
   <dimension ref="A1:B619"/>
   <sheetViews>
-    <sheetView topLeftCell="A331" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A556" sqref="A556"/>
+    <sheetView topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A291" sqref="A291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12391,7 +12464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF1E01E-01C2-7844-B628-8E09C0C92859}">
   <dimension ref="A1:B369"/>
   <sheetViews>
-    <sheetView topLeftCell="A350" workbookViewId="0">
+    <sheetView topLeftCell="A346" workbookViewId="0">
       <selection activeCell="A368" sqref="A368"/>
     </sheetView>
   </sheetViews>
@@ -15364,7 +15437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE85406E-B187-E14D-8DA8-2AAAAED9B666}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
@@ -16191,10 +16264,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99003BE-679F-9248-8C84-529C7407F5E3}">
-  <dimension ref="A1:B145"/>
+  <dimension ref="A1:B166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16212,647 +16285,647 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1645</v>
+        <v>1760</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1646</v>
+        <v>1758</v>
       </c>
       <c r="B3" t="s">
-        <v>284</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1647</v>
+        <v>1791</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1648</v>
+        <v>1775</v>
       </c>
       <c r="B5" t="s">
-        <v>1652</v>
+        <v>656</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1652</v>
+        <v>1764</v>
       </c>
       <c r="B6" t="s">
-        <v>1197</v>
+        <v>656</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1422</v>
+        <v>1789</v>
       </c>
       <c r="B7" t="s">
-        <v>1516</v>
+        <v>656</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1369</v>
+        <v>1711</v>
       </c>
       <c r="B8" t="s">
-        <v>1652</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>695</v>
+        <v>1739</v>
       </c>
       <c r="B9" t="s">
-        <v>697</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1653</v>
+        <v>1002</v>
       </c>
       <c r="B10" t="s">
-        <v>1654</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>517</v>
+        <v>1742</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1656</v>
+        <v>1753</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1657</v>
+        <v>1799</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1658</v>
+        <v>1770</v>
       </c>
       <c r="B14" t="s">
-        <v>1660</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1659</v>
+        <v>1670</v>
       </c>
       <c r="B15" t="s">
-        <v>284</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1661</v>
+        <v>1696</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1662</v>
+        <v>1700</v>
       </c>
       <c r="B17" t="s">
-        <v>1673</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1369</v>
+        <v>1662</v>
       </c>
       <c r="B18" t="s">
-        <v>1651</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1651</v>
+        <v>1718</v>
       </c>
       <c r="B19" t="s">
-        <v>517</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1663</v>
+        <v>1762</v>
       </c>
       <c r="B20" t="s">
-        <v>302</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1664</v>
+        <v>1774</v>
       </c>
       <c r="B21" t="s">
-        <v>302</v>
+        <v>470</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>370</v>
+        <v>1661</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1655</v>
+        <v>1744</v>
       </c>
       <c r="B23" t="s">
-        <v>1665</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1666</v>
+        <v>1725</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1667</v>
+        <v>1682</v>
       </c>
       <c r="B25" t="s">
-        <v>697</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>1668</v>
+        <v>1657</v>
       </c>
       <c r="B26" t="s">
-        <v>1669</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1669</v>
+        <v>1706</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>1670</v>
+        <v>1794</v>
       </c>
       <c r="B28" t="s">
-        <v>1650</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1671</v>
+        <v>1786</v>
       </c>
       <c r="B29" t="s">
-        <v>1670</v>
+        <v>540</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>1673</v>
+        <v>1795</v>
       </c>
       <c r="B30" t="s">
-        <v>1672</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>1674</v>
+        <v>1732</v>
       </c>
       <c r="B31" t="s">
-        <v>1669</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>1675</v>
+        <v>1787</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>1676</v>
+        <v>1727</v>
       </c>
       <c r="B33" t="s">
-        <v>1677</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>1678</v>
+        <v>1778</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>1679</v>
+        <v>1651</v>
       </c>
       <c r="B35" t="s">
-        <v>284</v>
+        <v>517</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>1558</v>
+        <v>1645</v>
       </c>
       <c r="B36" t="s">
-        <v>1651</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="B37" t="s">
-        <v>1651</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>1681</v>
+        <v>1687</v>
       </c>
       <c r="B38" t="s">
-        <v>1369</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1682</v>
+        <v>1768</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>1683</v>
+        <v>1747</v>
       </c>
       <c r="B40" t="s">
-        <v>1383</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>1684</v>
+        <v>1740</v>
       </c>
       <c r="B41" t="s">
-        <v>1686</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>1685</v>
+        <v>1781</v>
       </c>
       <c r="B42" t="s">
-        <v>1686</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>1687</v>
+        <v>1777</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>1687</v>
+        <v>1697</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>1688</v>
+        <v>1720</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>1689</v>
+        <v>1793</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>1649</v>
+        <v>1687</v>
       </c>
       <c r="B47" t="s">
-        <v>1369</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1690</v>
+        <v>1334</v>
       </c>
       <c r="B48" t="s">
-        <v>528</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1690</v>
+        <v>1647</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>1691</v>
+        <v>1666</v>
       </c>
       <c r="B50" t="s">
-        <v>346</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1692</v>
+        <v>1792</v>
       </c>
       <c r="B51" t="s">
-        <v>1385</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1693</v>
+        <v>1735</v>
       </c>
       <c r="B52" t="s">
-        <v>1658</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1694</v>
+        <v>1734</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>1695</v>
+        <v>1671</v>
       </c>
       <c r="B54" t="s">
-        <v>809</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>1696</v>
+        <v>1681</v>
       </c>
       <c r="B55" t="s">
-        <v>1650</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>1697</v>
+        <v>1649</v>
       </c>
       <c r="B56" t="s">
-        <v>1698</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1697</v>
+        <v>1709</v>
       </c>
       <c r="B57" t="s">
-        <v>1699</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>1699</v>
+        <v>1710</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>1700</v>
+        <v>1768</v>
       </c>
       <c r="B59" t="s">
-        <v>443</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1701</v>
+        <v>1790</v>
       </c>
       <c r="B60" t="s">
-        <v>1702</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1703</v>
+        <v>1801</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1704</v>
+        <v>1683</v>
       </c>
       <c r="B62" t="s">
-        <v>247</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1705</v>
+        <v>432</v>
       </c>
       <c r="B63" t="s">
-        <v>1715</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1706</v>
+        <v>1737</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="B65" t="s">
-        <v>18</v>
+        <v>247</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>1708</v>
+        <v>1703</v>
       </c>
       <c r="B66" t="s">
-        <v>398</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>1709</v>
+        <v>1749</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>1710</v>
+        <v>1729</v>
       </c>
       <c r="B68" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>1406</v>
+        <v>1716</v>
       </c>
       <c r="B69" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>1394</v>
+        <v>1689</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1711</v>
+        <v>1743</v>
       </c>
       <c r="B71" t="s">
-        <v>1468</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>1002</v>
+        <v>1697</v>
       </c>
       <c r="B72" t="s">
-        <v>1468</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>1628</v>
+        <v>1674</v>
       </c>
       <c r="B73" t="s">
-        <v>1712</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>1713</v>
+        <v>1668</v>
       </c>
       <c r="B74" t="s">
-        <v>1714</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>1716</v>
+        <v>1765</v>
       </c>
       <c r="B75" t="s">
-        <v>1242</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>1717</v>
+        <v>1712</v>
       </c>
       <c r="B76" t="s">
-        <v>16</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>1718</v>
+        <v>1788</v>
       </c>
       <c r="B77" t="s">
-        <v>850</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>1719</v>
+        <v>1646</v>
       </c>
       <c r="B78" t="s">
-        <v>1720</v>
+        <v>284</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>1721</v>
+        <v>1679</v>
       </c>
       <c r="B79" t="s">
-        <v>1687</v>
+        <v>284</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>1722</v>
+        <v>1659</v>
       </c>
       <c r="B80" t="s">
-        <v>1723</v>
+        <v>284</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>1724</v>
+        <v>1754</v>
       </c>
       <c r="B81" t="s">
-        <v>1546</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>1725</v>
+        <v>1688</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
@@ -16860,135 +16933,135 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>1633</v>
+        <v>1687</v>
       </c>
       <c r="B83" t="s">
-        <v>1689</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
       <c r="B84" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>1632</v>
+        <v>1802</v>
       </c>
       <c r="B85" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>1727</v>
+        <v>1756</v>
       </c>
       <c r="B86" t="s">
-        <v>1689</v>
+        <v>910</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>1728</v>
+        <v>1684</v>
       </c>
       <c r="B87" t="s">
-        <v>28</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>1729</v>
+        <v>1685</v>
       </c>
       <c r="B88" t="s">
-        <v>1385</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>1730</v>
+        <v>1628</v>
       </c>
       <c r="B89" t="s">
-        <v>16</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>1731</v>
+        <v>1745</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>1732</v>
+        <v>1699</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>1733</v>
+        <v>1664</v>
       </c>
       <c r="B92" t="s">
-        <v>1734</v>
+        <v>302</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>1735</v>
+        <v>1663</v>
       </c>
       <c r="B93" t="s">
-        <v>1737</v>
+        <v>302</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>1736</v>
+        <v>1750</v>
       </c>
       <c r="B94" t="s">
-        <v>1737</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>1738</v>
+        <v>1741</v>
       </c>
       <c r="B95" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>1739</v>
+        <v>1785</v>
       </c>
       <c r="B96" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>1740</v>
+        <v>1707</v>
       </c>
       <c r="B97" t="s">
-        <v>1468</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>1741</v>
+        <v>1406</v>
       </c>
       <c r="B98" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>1742</v>
+        <v>1780</v>
       </c>
       <c r="B99" t="s">
         <v>18</v>
@@ -16996,370 +17069,538 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>1743</v>
+        <v>1726</v>
       </c>
       <c r="B100" t="s">
-        <v>1468</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>1744</v>
+        <v>1633</v>
       </c>
       <c r="B101" t="s">
-        <v>16</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>1745</v>
+        <v>1694</v>
       </c>
       <c r="B102" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>1746</v>
+        <v>1761</v>
       </c>
       <c r="B103" t="s">
-        <v>1747</v>
+        <v>19</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>1748</v>
+        <v>1730</v>
       </c>
       <c r="B104" t="s">
-        <v>1749</v>
+        <v>19</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>1750</v>
+        <v>1738</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>1751</v>
+        <v>1731</v>
       </c>
       <c r="B106" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>1752</v>
+        <v>1632</v>
       </c>
       <c r="B107" t="s">
-        <v>1558</v>
+        <v>19</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>1753</v>
+        <v>1369</v>
       </c>
       <c r="B108" t="s">
-        <v>1405</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>1754</v>
+        <v>1648</v>
       </c>
       <c r="B109" t="s">
-        <v>1468</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>1755</v>
+        <v>1769</v>
       </c>
       <c r="B110" t="s">
-        <v>1756</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>1757</v>
+        <v>130</v>
       </c>
       <c r="B111" t="s">
-        <v>1758</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>1759</v>
+        <v>1317</v>
       </c>
       <c r="B112" t="s">
-        <v>1558</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>1760</v>
+        <v>1798</v>
       </c>
       <c r="B113" t="s">
-        <v>1761</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>1762</v>
+        <v>1369</v>
       </c>
       <c r="B114" t="s">
-        <v>1761</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>1334</v>
+        <v>1680</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>1763</v>
+        <v>1558</v>
       </c>
       <c r="B116" t="s">
-        <v>19</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>1764</v>
+        <v>1667</v>
       </c>
       <c r="B117" t="s">
-        <v>1765</v>
+        <v>697</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>1766</v>
+        <v>695</v>
       </c>
       <c r="B118" t="s">
-        <v>656</v>
+        <v>697</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>1767</v>
+        <v>1658</v>
       </c>
       <c r="B119" t="s">
-        <v>1768</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>1769</v>
+        <v>1784</v>
       </c>
       <c r="B120" t="s">
-        <v>27</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>1770</v>
+        <v>1776</v>
       </c>
       <c r="B121" t="s">
-        <v>52</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>1770</v>
+        <v>1652</v>
       </c>
       <c r="B122" t="s">
-        <v>3</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>130</v>
+        <v>1228</v>
       </c>
       <c r="B123" t="s">
-        <v>8</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>1771</v>
+        <v>1800</v>
       </c>
       <c r="B124" t="s">
-        <v>1773</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>1772</v>
+        <v>517</v>
       </c>
       <c r="B125" t="s">
-        <v>1774</v>
+        <v>30</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>1775</v>
+        <v>1690</v>
       </c>
       <c r="B126" t="s">
-        <v>324</v>
+        <v>30</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>1687</v>
+        <v>1701</v>
       </c>
       <c r="B127" t="s">
-        <v>3</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>1776</v>
+        <v>1656</v>
       </c>
       <c r="B128" t="s">
-        <v>470</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>1317</v>
+        <v>1799</v>
       </c>
       <c r="B129" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>1777</v>
+        <v>1705</v>
       </c>
       <c r="B130" t="s">
-        <v>656</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>432</v>
+        <v>1691</v>
       </c>
       <c r="B131" t="s">
-        <v>11</v>
+        <v>346</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>1778</v>
+        <v>1676</v>
       </c>
       <c r="B132" t="s">
-        <v>1197</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>1779</v>
+        <v>1721</v>
       </c>
       <c r="B133" t="s">
-        <v>130</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>1780</v>
+        <v>1693</v>
       </c>
       <c r="B134" t="s">
-        <v>28</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>1781</v>
+        <v>1796</v>
       </c>
       <c r="B135" t="s">
-        <v>1248</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>1782</v>
+        <v>1690</v>
       </c>
       <c r="B136" t="s">
-        <v>18</v>
+        <v>528</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>1230</v>
+        <v>370</v>
       </c>
       <c r="B137" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>1783</v>
+        <v>1717</v>
       </c>
       <c r="B138" t="s">
-        <v>130</v>
+        <v>850</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>1228</v>
+        <v>1728</v>
       </c>
       <c r="B139" t="s">
-        <v>1197</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>1784</v>
+        <v>1692</v>
       </c>
       <c r="B140" t="s">
-        <v>1785</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>1786</v>
+        <v>1752</v>
       </c>
       <c r="B141" t="s">
-        <v>1389</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>1787</v>
+        <v>1723</v>
       </c>
       <c r="B142" t="s">
-        <v>18</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>1788</v>
+        <v>1230</v>
       </c>
       <c r="B143" t="s">
-        <v>540</v>
+        <v>31</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>1789</v>
+        <v>1757</v>
       </c>
       <c r="B144" t="s">
-        <v>28</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>1790</v>
+        <v>1751</v>
       </c>
       <c r="B145" t="s">
-        <v>1208</v>
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B147" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B148" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B149" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B150" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B152" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B153" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B155" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B156" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B159" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B160" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B162" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B163" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B164" t="s">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B166" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>